<commit_message>
* Add voice channel to sound system.  * Update effect system.
</commit_message>
<xml_diff>
--- a/example/BuildSchema/Tables/SoundTable.xlsx
+++ b/example/BuildSchema/Tables/SoundTable.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Devwinsoft\devarc\example\BuildSchema\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D167249-6B64-461B-8E0D-7F8E4011337B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE485F81-11E9-47D8-A00F-1D43D38D7CE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{84FD4B15-AE04-431D-A01B-7BE3057C75B0}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="27">
   <si>
     <t>string</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -136,6 +136,14 @@
   </si>
   <si>
     <t>loading identifier</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>cooltime</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sound Cooltime</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -213,11 +221,17 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -239,9 +253,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 테마">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -279,7 +293,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -385,7 +399,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -527,7 +541,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -535,7 +549,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3401DA0E-6D94-4657-8FD9-3F778EFEE5A9}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -545,9 +559,10 @@
     <col min="3" max="3" width="20.875" customWidth="1"/>
     <col min="4" max="4" width="10.125" customWidth="1"/>
     <col min="5" max="5" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -563,8 +578,11 @@
       <c r="E1" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F1" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -580,8 +598,11 @@
       <c r="E2" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F2" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -597,16 +618,20 @@
       <c r="E3" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F3" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>10001</v>
       </c>
@@ -622,8 +647,11 @@
       <c r="E5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F5" s="3">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>10002</v>
       </c>
@@ -639,8 +667,11 @@
       <c r="E6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F6" s="3">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>10003</v>
       </c>
@@ -655,6 +686,9 @@
       </c>
       <c r="E7">
         <v>1</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0.05</v>
       </c>
     </row>
   </sheetData>
@@ -665,7 +699,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C2B1D51-3465-4341-8DCF-974BA4470843}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -676,9 +710,10 @@
     <col min="4" max="4" width="21.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -697,8 +732,11 @@
       <c r="F1" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G1" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -717,8 +755,11 @@
       <c r="F2" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G2" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -737,16 +778,20 @@
       <c r="F3" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G3" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -765,8 +810,11 @@
       <c r="F5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G5" s="3">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2</v>
       </c>
@@ -781,6 +829,9 @@
       </c>
       <c r="F6">
         <v>1</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0.05</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
* Add 3d sound roll off function.
</commit_message>
<xml_diff>
--- a/example/BuildSchema/Tables/SoundTable.xlsx
+++ b/example/BuildSchema/Tables/SoundTable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Devwinsoft\devarc\example\BuildSchema\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE485F81-11E9-47D8-A00F-1D43D38D7CE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{399DBD71-6D1D-4741-9D78-5C187E136F68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{84FD4B15-AE04-431D-A01B-7BE3057C75B0}"/>
+    <workbookView xWindow="1575" yWindow="600" windowWidth="25635" windowHeight="13905" xr2:uid="{84FD4B15-AE04-431D-A01B-7BE3057C75B0}"/>
   </bookViews>
   <sheets>
     <sheet name="SOUND_BUNDLE" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="29">
   <si>
     <t>string</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -144,6 +144,14 @@
   </si>
   <si>
     <t>Sound Cooltime</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>area_close</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>area_far</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -549,9 +557,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3401DA0E-6D94-4657-8FD9-3F778EFEE5A9}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6:H6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -562,7 +572,7 @@
     <col min="6" max="6" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -582,7 +592,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -601,8 +611,14 @@
       <c r="F2" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -621,8 +637,14 @@
       <c r="F3" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -631,7 +653,7 @@
       </c>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>10001</v>
       </c>
@@ -650,8 +672,14 @@
       <c r="F5" s="3">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G5">
+        <v>20</v>
+      </c>
+      <c r="H5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>10002</v>
       </c>
@@ -670,8 +698,14 @@
       <c r="F6" s="3">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G6">
+        <v>20</v>
+      </c>
+      <c r="H6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>10003</v>
       </c>
@@ -689,6 +723,12 @@
       </c>
       <c r="F7" s="3">
         <v>0.05</v>
+      </c>
+      <c r="G7">
+        <v>20</v>
+      </c>
+      <c r="H7">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -699,9 +739,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C2B1D51-3465-4341-8DCF-974BA4470843}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -713,7 +753,7 @@
     <col min="7" max="7" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -736,7 +776,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -758,8 +798,14 @@
       <c r="G2" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -781,8 +827,14 @@
       <c r="G3" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -791,7 +843,7 @@
       </c>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -814,7 +866,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
* Add SoundManager functions.  - Mute function.  - Changing volumn.
</commit_message>
<xml_diff>
--- a/example/BuildSchema/Tables/SoundTable.xlsx
+++ b/example/BuildSchema/Tables/SoundTable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Devwinsoft\devarc\example\BuildSchema\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{399DBD71-6D1D-4741-9D78-5C187E136F68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80F247FC-4F4A-4B0E-893C-F04D2E1DD810}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1575" yWindow="600" windowWidth="25635" windowHeight="13905" xr2:uid="{84FD4B15-AE04-431D-A01B-7BE3057C75B0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{84FD4B15-AE04-431D-A01B-7BE3057C75B0}"/>
   </bookViews>
   <sheets>
     <sheet name="SOUND_BUNDLE" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="27">
   <si>
     <t>string</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -84,14 +84,6 @@
   </si>
   <si>
     <t>float</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>volume</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Default Volume</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -557,24 +549,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3401DA0E-6D94-4657-8FD9-3F778EFEE5A9}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6:H6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="17.75" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.875" customWidth="1"/>
     <col min="4" max="4" width="10.125" customWidth="1"/>
-    <col min="5" max="5" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9" style="3"/>
+    <col min="5" max="5" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>3</v>
@@ -585,16 +574,13 @@
       <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E1" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
@@ -605,22 +591,19 @@
       <c r="D2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="2" t="s">
+      <c r="E2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>25</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>0</v>
@@ -631,7 +614,7 @@
       <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -640,94 +623,82 @@
       <c r="G3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>10001</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D5" t="b">
         <v>0</v>
       </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5" s="3">
+      <c r="E5" s="3">
         <v>0.05</v>
       </c>
+      <c r="F5">
+        <v>20</v>
+      </c>
       <c r="G5">
-        <v>20</v>
-      </c>
-      <c r="H5">
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>10002</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D6" t="b">
         <v>0</v>
       </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6" s="3">
+      <c r="E6" s="3">
         <v>0.05</v>
       </c>
+      <c r="F6">
+        <v>20</v>
+      </c>
       <c r="G6">
-        <v>20</v>
-      </c>
-      <c r="H6">
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>10003</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D7" t="b">
         <v>0</v>
       </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7" s="3">
+      <c r="E7" s="3">
         <v>0.05</v>
       </c>
+      <c r="F7">
+        <v>20</v>
+      </c>
       <c r="G7">
-        <v>20</v>
-      </c>
-      <c r="H7">
         <v>50</v>
       </c>
     </row>
@@ -739,9 +710,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C2B1D51-3465-4341-8DCF-974BA4470843}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -749,16 +720,15 @@
     <col min="3" max="3" width="12.25" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9" style="3"/>
+    <col min="6" max="6" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3</v>
@@ -769,16 +739,13 @@
       <c r="E1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F1" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
@@ -792,22 +759,19 @@
       <c r="E2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="2" t="s">
+      <c r="F2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>25</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>0</v>
@@ -821,7 +785,7 @@
       <c r="E3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="G3" s="2" t="s">
@@ -830,43 +794,37 @@
       <c r="H3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E5" t="b">
         <v>1</v>
       </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5" s="3">
+      <c r="F5" s="3">
         <v>0.05</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2</v>
       </c>
@@ -874,15 +832,12 @@
         <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E6" t="b">
         <v>0</v>
       </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="G6" s="3">
+      <c r="F6" s="3">
         <v>0.05</v>
       </c>
     </row>

</xml_diff>